<commit_message>
pros-15500 GSKJP CR - moved dev work to psapac-sand3
</commit_message>
<xml_diff>
--- a/Projects/PSAPAC_SAND3/Data/gsk_set_up.xlsx
+++ b/Projects/PSAPAC_SAND3/Data/gsk_set_up.xlsx
@@ -15,7 +15,7 @@
   </externalReferences>
   <definedNames>
     <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$J$3</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$J$4</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="31">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -65,10 +65,10 @@
     <t xml:space="preserve">Include POSM</t>
   </si>
   <si>
-    <t xml:space="preserve">Facings SOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pain Main Shelf, Oral Main Shelf, Respiratory Main Shelf, NRT Main Shelf, Other Main Shelf, Pain Main Shelf - Grcy, Oral Main Shelf - Grcy, NRT Main Shelf – Grcy, Wellness Main Shelf, Wellness Main Shelf - Grcy</t>
+    <t xml:space="preserve">Linear SOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oral Main Shelf</t>
   </si>
   <si>
     <t xml:space="preserve">Exclude</t>
@@ -77,16 +77,49 @@
     <t xml:space="preserve">Include</t>
   </si>
   <si>
-    <t xml:space="preserve">Adult,Child,Denture,NRT,Toothpaste,Topical,Osteo,Pain Other,Respiratory Other</t>
+    <t xml:space="preserve">Oral Care</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tooth paste,Denture cleanser,Denture adhesive</t>
   </si>
   <si>
     <t xml:space="preserve">Availability</t>
   </si>
   <si>
-    <t xml:space="preserve">Include </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linear SOS</t>
+    <t xml:space="preserve">Oral Main Shelf, CCA Main Shelf, Pain Relief Main Shelf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oral Care, Respiratory and Skin Health, Pain relief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tooth paste,Denture cleanser,Denture adhesive, Allergy, Cold &amp; Flu, Pain Relief</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSK_PLN_MSL_SCORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shumitect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tooth paste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSK_PLN_LSOS_SCORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSK_PLN_BLOCK_SCORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSK_PLN_POSITION_SCORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GSK_ECAPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End Cap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">POSM</t>
   </si>
 </sst>
 </file>
@@ -150,8 +183,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FFDDDDDD"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
   </fills>
@@ -203,7 +236,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -225,11 +258,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -237,19 +270,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -257,15 +278,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -302,7 +319,7 @@
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
       <rgbColor rgb="FF0066CC"/>
-      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FFDDDDDD"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -351,31 +368,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:AMJ9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="E2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="95.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="24.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="49.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="13.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="23.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="11.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="31.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="9.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1014" min="13" style="1" width="8.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1015" style="0" width="8.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="22.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.02"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="43.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="30.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1014" min="12" style="1" width="8.79"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1015" style="0" width="8.79"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="45.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="46" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -412,99 +431,237 @@
       <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" s="5" customFormat="true" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="AMA1" s="0"/>
+      <c r="AMB1" s="0"/>
+      <c r="AMC1" s="0"/>
+      <c r="AMD1" s="0"/>
+      <c r="AME1" s="0"/>
+      <c r="AMF1" s="0"/>
+      <c r="AMG1" s="0"/>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" s="8" customFormat="true" ht="29.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="7" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>14</v>
+      <c r="D2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L2" s="9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="K2" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="7" t="s">
+      <c r="L2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="AMA2" s="0"/>
+      <c r="AMB2" s="0"/>
+      <c r="AMC2" s="0"/>
+      <c r="AMD2" s="0"/>
+      <c r="AME2" s="0"/>
+      <c r="AMF2" s="0"/>
+      <c r="AMG2" s="0"/>
+      <c r="AMH2" s="0"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row r="3" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="8"/>
+      <c r="C3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="10"/>
+      <c r="H3" s="8"/>
+      <c r="J3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="8"/>
+      <c r="C4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="0"/>
-      <c r="I3" s="0"/>
-      <c r="J3" s="0"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="11" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="12" t="s">
+      <c r="D4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="10"/>
+      <c r="H4" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L4" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="8"/>
+      <c r="C5" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="14.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="L7" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="14.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="8"/>
+      <c r="J8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="L8" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="B4" s="13"/>
-      <c r="C4" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="15"/>
-      <c r="I4" s="15"/>
-      <c r="J4" s="15"/>
-      <c r="K4" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>